<commit_message>
add export du datas
</commit_message>
<xml_diff>
--- a/templates/毒app抓取数据_template.xlsx
+++ b/templates/毒app抓取数据_template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>&lt;%=eny.title%&gt;</t>
   </si>
@@ -78,22 +78,56 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>销量</t>
+    <t>&lt;%=eny.price%&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%forRow eny in _data_%&gt;&lt;%=eny.sku%&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=eny.soldTotal%&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>总销量</t>
     <rPh sb="0" eb="1">
+      <t>zong</t>
+    </rPh>
+    <rPh sb="1" eb="2">
       <t>xiao liang</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;%=eny.price%&gt;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%forRow eny in _data_%&gt;&lt;%=eny.sku%&gt;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=eny.sold_total%&gt;</t>
+    <t>&lt;%=eny.soldDetail%&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>前一天销量</t>
+    <rPh sb="0" eb="1">
+      <t>qian yi tian</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>xiao liang</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=eny.soldNum%&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>前一天尺码销量</t>
+    <rPh sb="0" eb="1">
+      <t>qian yi tian</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>chi ma</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>xiao liang</t>
+    </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -482,11 +516,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -497,7 +531,7 @@
     <col min="4" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -511,12 +545,18 @@
         <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -525,10 +565,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>